<commit_message>
Added ability to query for country group to the population source
</commit_message>
<xml_diff>
--- a/sources/unpd/data/UN_PPP2019_PopTot.xlsx
+++ b/sources/unpd/data/UN_PPP2019_PopTot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomas/Dropbox/Coding/datascrapper2/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomas.Gonzalez\datascrapper2\sources\unpd\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0A9229-54A8-A143-A157-B400F90A736E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8670FB7-64F2-49DC-874D-E66E426DEC9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25320" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="25320" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Median" sheetId="3" r:id="rId1"/>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="294">
   <si>
-    <t>Region, subregion, country or area</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -906,6 +903,9 @@
   </si>
   <si>
     <t>United States of America</t>
+  </si>
+  <si>
+    <t>entity</t>
   </si>
 </sst>
 </file>
@@ -1407,23 +1407,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S286"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.25" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="61.75" customWidth="1"/>
-    <col min="2" max="2" width="19.75" customWidth="1"/>
-    <col min="3" max="19" width="13.75" customWidth="1"/>
+    <col min="1" max="1" width="61.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="19" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="4">
         <v>2020</v>
@@ -1477,12 +1475,12 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3">
         <v>7794798.7290000003</v>
@@ -1536,12 +1534,12 @@
         <v>10875393.719000001</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>5</v>
       </c>
       <c r="C3" s="3">
         <v>1273304.2609999999</v>
@@ -1595,12 +1593,12 @@
         <v>1244295.6200000001</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3">
         <v>6521494.4680000003</v>
@@ -1654,12 +1652,12 @@
         <v>9631098.0989999995</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3">
         <v>1057438.1629999999</v>
@@ -1713,12 +1711,12 @@
         <v>3046778.7829999998</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="3">
         <v>5464056.3049999997</v>
@@ -1772,12 +1770,12 @@
         <v>6584319.3159999996</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="3">
         <v>5050207.5889999997</v>
@@ -1831,12 +1829,12 @@
         <v>8541186.9370000008</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="C8" s="3">
         <v>533143.39800000004</v>
@@ -1890,12 +1888,12 @@
         <v>1405998.426</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3">
         <v>72076.097999999998</v>
@@ -1949,12 +1947,12 @@
         <v>87598.837</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="C10" s="3">
         <v>1263092.9339999999</v>
@@ -2008,12 +2006,12 @@
         <v>1303541.3189999999</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3">
         <v>5753051.6150000002</v>
@@ -2067,12 +2065,12 @@
         <v>7082398.8059999999</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="3">
         <v>2654816.3309999998</v>
@@ -2126,12 +2124,12 @@
         <v>2380613.2570000002</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="3">
         <v>3098235.284</v>
@@ -2185,12 +2183,12 @@
         <v>4701785.5489999996</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="3">
         <v>775710.61199999996</v>
@@ -2244,12 +2242,12 @@
         <v>2484829.25</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="3">
         <v>2943.5680000000002</v>
@@ -2303,12 +2301,12 @@
         <v>4624.3440000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="C16" s="3">
         <v>1340598.1129999999</v>
@@ -2362,12 +2360,12 @@
         <v>4280127.1310000001</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3">
         <v>4641054.7860000003</v>
@@ -2421,12 +2419,12 @@
         <v>4719906.92</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="3">
         <v>747636.04500000004</v>
@@ -2480,12 +2478,12 @@
         <v>629562.56200000003</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="3">
         <v>653962.33200000005</v>
@@ -2539,12 +2537,12 @@
         <v>679992.94</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="3">
         <v>368869.64399999997</v>
@@ -2598,12 +2596,12 @@
         <v>490888.55599999998</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="3">
         <v>42677.809000000001</v>
@@ -2657,12 +2655,12 @@
         <v>74915.61</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="C22" s="3">
         <v>1094365.605</v>
@@ -2716,12 +2714,12 @@
         <v>3775269.514</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="C23" s="3">
         <v>445405.57799999998</v>
@@ -2775,12 +2773,12 @@
         <v>1451842.4920000001</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="3">
         <v>11890.781000000001</v>
@@ -2834,12 +2832,12 @@
         <v>50904.072</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" s="3">
         <v>869.59500000000003</v>
@@ -2893,12 +2891,12 @@
         <v>2186.509</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" s="3">
         <v>988.00199999999995</v>
@@ -2952,12 +2950,12 @@
         <v>1331.6559999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27" s="3">
         <v>3546.4270000000001</v>
@@ -3011,12 +3009,12 @@
         <v>9061.777</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" s="3">
         <v>114963.583</v>
@@ -3070,12 +3068,12 @@
         <v>294392.90299999999</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" s="3">
         <v>53771.3</v>
@@ -3129,12 +3127,12 @@
         <v>125423.855</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="3">
         <v>27691.019</v>
@@ -3188,12 +3186,12 @@
         <v>99957.34</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" s="3">
         <v>19129.955000000002</v>
@@ -3247,12 +3245,12 @@
         <v>66559.385999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" s="3">
         <v>1271.7670000000001</v>
@@ -3306,12 +3304,12 @@
         <v>827.303</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" s="3">
         <v>272.81299999999999</v>
@@ -3365,12 +3363,12 @@
         <v>745.69100000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34" s="3">
         <v>31255.435000000001</v>
@@ -3424,12 +3422,12 @@
         <v>123646.947</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" s="3">
         <v>895.30799999999999</v>
@@ -3483,12 +3481,12 @@
         <v>901.24900000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" s="3">
         <v>12952.209000000001</v>
@@ -3542,12 +3540,12 @@
         <v>33412.642999999996</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C37" s="3">
         <v>98.34</v>
@@ -3601,12 +3599,12 @@
         <v>88.326999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C38" s="3">
         <v>15893.218999999999</v>
@@ -3660,12 +3658,12 @@
         <v>75716.429000000004</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C39" s="3">
         <v>11193.728999999999</v>
@@ -3719,12 +3717,12 @@
         <v>31738.063999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C40" s="3">
         <v>45741</v>
@@ -3778,12 +3776,12 @@
         <v>136784.87599999999</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C41" s="3">
         <v>59734.213000000003</v>
@@ -3837,12 +3835,12 @@
         <v>285651.84600000002</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C42" s="3">
         <v>18383.955999999998</v>
@@ -3896,12 +3894,12 @@
         <v>81546.198000000004</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C43" s="3">
         <v>14862.927</v>
@@ -3955,12 +3953,12 @@
         <v>30965.420999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C44" s="3">
         <v>179595.125</v>
@@ -4014,12 +4012,12 @@
         <v>746060.56200000003</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C45" s="3">
         <v>32866.267999999996</v>
@@ -4073,12 +4071,12 @@
         <v>188283.13200000001</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C46" s="3">
         <v>26545.864000000001</v>
@@ -4132,12 +4130,12 @@
         <v>90225.178</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C47" s="3">
         <v>4829.7640000000001</v>
@@ -4191,12 +4189,12 @@
         <v>11631.41</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C48" s="3">
         <v>16425.859</v>
@@ -4250,12 +4248,12 @@
         <v>61849.82</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C49" s="3">
         <v>5518.0919999999996</v>
@@ -4309,12 +4307,12 @@
         <v>20961.987000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C50" s="3">
         <v>89561.403999999995</v>
@@ -4368,12 +4366,12 @@
         <v>362031.08199999999</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C51" s="3">
         <v>1402.9849999999999</v>
@@ -4427,12 +4425,12 @@
         <v>4510.6310000000003</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C52" s="3">
         <v>2225.7280000000001</v>
@@ -4486,12 +4484,12 @@
         <v>5859.2250000000004</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C53" s="3">
         <v>219.161</v>
@@ -4545,12 +4543,12 @@
         <v>708.09699999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C54" s="3">
         <v>67503.646999999997</v>
@@ -4604,12 +4602,12 @@
         <v>93570.918000000005</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C55" s="3">
         <v>2351.625</v>
@@ -4663,12 +4661,12 @@
         <v>4165.8609999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C56" s="3">
         <v>1160.164</v>
@@ -4722,12 +4720,12 @@
         <v>2145.1979999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C57" s="3">
         <v>2142.252</v>
@@ -4781,12 +4779,12 @@
         <v>2695.4380000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C58" s="3">
         <v>2540.9160000000002</v>
@@ -4840,12 +4838,12 @@
         <v>5373.5889999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C59" s="3">
         <v>59308.69</v>
@@ -4899,12 +4897,12 @@
         <v>79190.831999999995</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C60" s="3">
         <v>401861.255</v>
@@ -4958,12 +4956,12 @@
         <v>1483795.5419999999</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C61" s="3">
         <v>12123.198</v>
@@ -5017,12 +5015,12 @@
         <v>47208.998</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C62" s="3">
         <v>20903.277999999998</v>
@@ -5076,12 +5074,12 @@
         <v>83194.232999999993</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C63" s="3">
         <v>555.98800000000006</v>
@@ -5135,12 +5133,12 @@
         <v>603.94899999999996</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C64" s="3">
         <v>26378.275000000001</v>
@@ -5194,12 +5192,12 @@
         <v>96632.721000000005</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C65" s="3">
         <v>2416.6640000000002</v>
@@ -5253,12 +5251,12 @@
         <v>8175.5529999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C66" s="3">
         <v>31072.945</v>
@@ -5312,12 +5310,12 @@
         <v>79011.409</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C67" s="3">
         <v>13132.791999999999</v>
@@ -5371,12 +5369,12 @@
         <v>45256.875999999997</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C68" s="3">
         <v>1967.998</v>
@@ -5430,12 +5428,12 @@
         <v>5706.2889999999998</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C69" s="3">
         <v>5057.6769999999997</v>
@@ -5489,12 +5487,12 @@
         <v>15525.036</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C70" s="3">
         <v>20250.833999999999</v>
@@ -5548,12 +5546,12 @@
         <v>80382.697</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C71" s="3">
         <v>4649.66</v>
@@ -5607,12 +5605,12 @@
         <v>17064.607</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C72" s="3">
         <v>24206.635999999999</v>
@@ -5666,12 +5664,12 @@
         <v>164947.337</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C73" s="3">
         <v>206139.587</v>
@@ -5725,12 +5723,12 @@
         <v>732941.59600000002</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C74" s="3">
         <v>6.0709999999999997</v>
@@ -5784,12 +5782,12 @@
         <v>4.4960000000000004</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C75" s="3">
         <v>16743.93</v>
@@ -5843,12 +5841,12 @@
         <v>63515.357000000004</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C76" s="3">
         <v>7976.9849999999997</v>
@@ -5902,12 +5900,12 @@
         <v>16675.197</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C77" s="3">
         <v>8278.7369999999992</v>
@@ -5961,12 +5959,12 @@
         <v>26949.190999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A78" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C78" s="3">
         <v>525869.28200000001</v>
@@ -6020,12 +6018,12 @@
         <v>927826.76100000006</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C79" s="3">
         <v>246232.508</v>
@@ -6079,12 +6077,12 @@
         <v>504857.61700000003</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A80" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C80" s="3">
         <v>43851.042999999998</v>
@@ -6138,12 +6136,12 @@
         <v>70704.619000000006</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C81" s="3">
         <v>102334.40300000001</v>
@@ -6197,12 +6195,12 @@
         <v>224735.18</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C82" s="3">
         <v>6871.2870000000003</v>
@@ -6256,12 +6254,12 @@
         <v>8011.54</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C83" s="3">
         <v>36910.557999999997</v>
@@ -6315,12 +6313,12 @@
         <v>44707.864000000001</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A84" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C84" s="3">
         <v>43849.269</v>
@@ -6374,12 +6372,12 @@
         <v>142342.356</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C85" s="3">
         <v>11818.618</v>
@@ -6433,12 +6431,12 @@
         <v>12972.285</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C86" s="3">
         <v>597.33000000000004</v>
@@ -6492,12 +6490,12 @@
         <v>1383.7729999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C87" s="3">
         <v>279636.77399999998</v>
@@ -6551,12 +6549,12 @@
         <v>422969.14399999997</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C88" s="3">
         <v>2963.2339999999999</v>
@@ -6610,12 +6608,12 @@
         <v>2038.6130000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C89" s="3">
         <v>10139.174999999999</v>
@@ -6669,12 +6667,12 @@
         <v>9192.1409999999996</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A90" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C90" s="3">
         <v>1701.5830000000001</v>
@@ -6728,12 +6726,12 @@
         <v>2251.8910000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C91" s="3">
         <v>1207.3610000000001</v>
@@ -6787,12 +6785,12 @@
         <v>1308.9110000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C92" s="3">
         <v>3989.1750000000002</v>
@@ -6846,12 +6844,12 @@
         <v>2514.13</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C93" s="3">
         <v>40222.502999999997</v>
@@ -6905,12 +6903,12 @@
         <v>107711.273</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A94" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C94" s="3">
         <v>8655.5409999999993</v>
@@ -6964,12 +6962,12 @@
         <v>18127.523000000001</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C95" s="3">
         <v>10203.14</v>
@@ -7023,12 +7021,12 @@
         <v>13644.11</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A96" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C96" s="3">
         <v>4270.5630000000001</v>
@@ -7082,12 +7080,12 @@
         <v>6188.9830000000002</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A97" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C97" s="3">
         <v>6825.442</v>
@@ -7141,12 +7139,12 @@
         <v>5707.2089999999998</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A98" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C98" s="3">
         <v>5106.6220000000003</v>
@@ -7200,12 +7198,12 @@
         <v>7267.893</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A99" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C99" s="3">
         <v>2881.06</v>
@@ -7259,12 +7257,12 @@
         <v>4162.4080000000004</v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A100" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C100" s="3">
         <v>34813.866999999998</v>
@@ -7318,12 +7316,12 @@
         <v>42231.012000000002</v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A101" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C101" s="3">
         <v>5101.4160000000002</v>
@@ -7377,12 +7375,12 @@
         <v>12268.218000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A102" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C102" s="3">
         <v>17500.656999999999</v>
@@ -7436,12 +7434,12 @@
         <v>36103.178</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A103" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C103" s="3">
         <v>84339.066999999995</v>
@@ -7495,12 +7493,12 @@
         <v>86170.462</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A104" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C104" s="3">
         <v>9890.4</v>
@@ -7554,12 +7552,12 @@
         <v>12909.869000000001</v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A105" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C105" s="3">
         <v>29825.968000000001</v>
@@ -7613,12 +7611,12 @@
         <v>53171.32</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A106" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C106" s="3">
         <v>2014708.531</v>
@@ -7672,12 +7670,12 @@
         <v>2330130.12</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A107" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C107" s="3">
         <v>74338.926000000007</v>
@@ -7731,12 +7729,12 @@
         <v>114922.97</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A108" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C108" s="3">
         <v>18776.706999999999</v>
@@ -7790,12 +7788,12 @@
         <v>27917.814999999999</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A109" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C109" s="3">
         <v>6524.1909999999998</v>
@@ -7849,12 +7847,12 @@
         <v>10984.938</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A110" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C110" s="3">
         <v>9537.6419999999998</v>
@@ -7908,12 +7906,12 @@
         <v>25328.026000000002</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C111" s="3">
         <v>6031.1869999999999</v>
@@ -7967,12 +7965,12 @@
         <v>8421.3490000000002</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A112" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C112" s="3">
         <v>33469.199000000001</v>
@@ -8026,12 +8024,12 @@
         <v>42270.841999999997</v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A113" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C113" s="3">
         <v>1940369.605</v>
@@ -8085,12 +8083,12 @@
         <v>2215207.15</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A114" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C114" s="3">
         <v>38928.341</v>
@@ -8144,12 +8142,12 @@
         <v>74937.960999999996</v>
       </c>
     </row>
-    <row r="115" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A115" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C115" s="3">
         <v>164689.383</v>
@@ -8203,12 +8201,12 @@
         <v>151393.01800000001</v>
       </c>
     </row>
-    <row r="116" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A116" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C116" s="3">
         <v>771.61199999999997</v>
@@ -8262,12 +8260,12 @@
         <v>686.28700000000003</v>
       </c>
     </row>
-    <row r="117" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A117" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C117" s="3">
         <v>1380004.385</v>
@@ -8321,12 +8319,12 @@
         <v>1447025.612</v>
       </c>
     </row>
-    <row r="118" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A118" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C118" s="3">
         <v>83992.952999999994</v>
@@ -8380,12 +8378,12 @@
         <v>98587.985000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A119" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C119" s="3">
         <v>540.54200000000003</v>
@@ -8439,12 +8437,12 @@
         <v>490.05799999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A120" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C120" s="3">
         <v>29136.808000000001</v>
@@ -8498,12 +8496,12 @@
         <v>23708.192999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A121" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C121" s="3">
         <v>220892.33100000001</v>
@@ -8557,12 +8555,12 @@
         <v>403102.82699999999</v>
       </c>
     </row>
-    <row r="122" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A122" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C122" s="3">
         <v>21413.25</v>
@@ -8616,12 +8614,12 @@
         <v>15275.209000000001</v>
       </c>
     </row>
-    <row r="123" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A123" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C123" s="3">
         <v>2346709.4810000001</v>
@@ -8675,12 +8673,12 @@
         <v>1966807.656</v>
       </c>
     </row>
-    <row r="124" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A124" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C124" s="3">
         <v>1678089.6270000001</v>
@@ -8734,12 +8732,12 @@
         <v>1222592.534</v>
       </c>
     </row>
-    <row r="125" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A125" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C125" s="3">
         <v>1439323.774</v>
@@ -8793,12 +8791,12 @@
         <v>1064993.4569999999</v>
       </c>
     </row>
-    <row r="126" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A126" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C126" s="3">
         <v>7496.9880000000003</v>
@@ -8852,12 +8850,12 @@
         <v>7647.2309999999998</v>
       </c>
     </row>
-    <row r="127" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A127" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C127" s="3">
         <v>649.34199999999998</v>
@@ -8911,12 +8909,12 @@
         <v>1011.617</v>
       </c>
     </row>
-    <row r="128" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A128" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C128" s="3">
         <v>23816.775000000001</v>
@@ -8970,12 +8968,12 @@
         <v>16258.857</v>
       </c>
     </row>
-    <row r="129" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A129" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C129" s="3">
         <v>25778.814999999999</v>
@@ -9029,12 +9027,12 @@
         <v>22792.832999999999</v>
       </c>
     </row>
-    <row r="130" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A130" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C130" s="3">
         <v>126476.458</v>
@@ -9088,12 +9086,12 @@
         <v>74959.377999999997</v>
       </c>
     </row>
-    <row r="131" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A131" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C131" s="3">
         <v>3278.2919999999999</v>
@@ -9147,12 +9145,12 @@
         <v>5387.2079999999996</v>
       </c>
     </row>
-    <row r="132" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A132" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C132" s="3">
         <v>51269.182999999997</v>
@@ -9206,12 +9204,12 @@
         <v>29541.953000000001</v>
       </c>
     </row>
-    <row r="133" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A133" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C133" s="3">
         <v>668619.85400000005</v>
@@ -9265,12 +9263,12 @@
         <v>744215.12199999997</v>
       </c>
     </row>
-    <row r="134" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A134" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C134" s="3">
         <v>437.483</v>
@@ -9324,12 +9322,12 @@
         <v>389.88400000000001</v>
       </c>
     </row>
-    <row r="135" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A135" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C135" s="3">
         <v>16718.971000000001</v>
@@ -9383,12 +9381,12 @@
         <v>21355.010999999999</v>
       </c>
     </row>
-    <row r="136" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A136" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C136" s="3">
         <v>273523.62099999998</v>
@@ -9442,12 +9440,12 @@
         <v>320782.42599999998</v>
       </c>
     </row>
-    <row r="137" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A137" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C137" s="3">
         <v>7275.5559999999996</v>
@@ -9501,12 +9499,12 @@
         <v>8423.9779999999992</v>
       </c>
     </row>
-    <row r="138" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A138" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C138" s="3">
         <v>32365.998</v>
@@ -9560,12 +9558,12 @@
         <v>40078.167000000001</v>
       </c>
     </row>
-    <row r="139" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A139" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C139" s="3">
         <v>54409.794000000002</v>
@@ -9619,12 +9617,12 @@
         <v>55298.928999999996</v>
       </c>
     </row>
-    <row r="140" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A140" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C140" s="3">
         <v>109581.08500000001</v>
@@ -9678,12 +9676,12 @@
         <v>146327.44099999999</v>
       </c>
     </row>
-    <row r="141" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A141" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C141" s="3">
         <v>5850.3429999999998</v>
@@ -9737,12 +9735,12 @@
         <v>5733.4769999999999</v>
       </c>
     </row>
-    <row r="142" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A142" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C142" s="3">
         <v>69799.978000000003</v>
@@ -9796,12 +9794,12 @@
         <v>46015.553</v>
       </c>
     </row>
-    <row r="143" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A143" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C143" s="3">
         <v>1318.442</v>
@@ -9855,12 +9853,12 @@
         <v>2372.9699999999998</v>
       </c>
     </row>
-    <row r="144" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A144" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C144" s="3">
         <v>97338.582999999999</v>
@@ -9914,12 +9912,12 @@
         <v>97437.285999999993</v>
       </c>
     </row>
-    <row r="145" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A145" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C145" s="3">
         <v>653962.33200000005</v>
@@ -9973,12 +9971,12 @@
         <v>679992.94</v>
       </c>
     </row>
-    <row r="146" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A146" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C146" s="3">
         <v>43532.374000000003</v>
@@ -10032,12 +10030,12 @@
         <v>38838.008999999998</v>
       </c>
     </row>
-    <row r="147" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A147" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C147" s="3">
         <v>15.002000000000001</v>
@@ -10091,12 +10089,12 @@
         <v>13.635</v>
       </c>
     </row>
-    <row r="148" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A148" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C148" s="3">
         <v>97.927999999999997</v>
@@ -10150,12 +10148,12 @@
         <v>102.048</v>
       </c>
     </row>
-    <row r="149" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A149" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C149" s="3">
         <v>106.76600000000001</v>
@@ -10209,12 +10207,12 @@
         <v>102.235</v>
       </c>
     </row>
-    <row r="150" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A150" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C150" s="3">
         <v>393.24799999999999</v>
@@ -10268,12 +10266,12 @@
         <v>460.11599999999999</v>
       </c>
     </row>
-    <row r="151" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A151" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C151" s="3">
         <v>287.37099999999998</v>
@@ -10327,12 +10325,12 @@
         <v>214.78800000000001</v>
       </c>
     </row>
-    <row r="152" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A152" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C152" s="3">
         <v>26.221</v>
@@ -10386,12 +10384,12 @@
         <v>32.606000000000002</v>
       </c>
     </row>
-    <row r="153" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A153" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C153" s="3">
         <v>30.236999999999998</v>
@@ -10445,12 +10443,12 @@
         <v>24.856999999999999</v>
       </c>
     </row>
-    <row r="154" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A154" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C154" s="3">
         <v>65.72</v>
@@ -10504,12 +10502,12 @@
         <v>102.667</v>
       </c>
     </row>
-    <row r="155" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A155" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C155" s="3">
         <v>11326.616</v>
@@ -10563,12 +10561,12 @@
         <v>6671.4610000000002</v>
       </c>
     </row>
-    <row r="156" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A156" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C156" s="3">
         <v>164.1</v>
@@ -10622,12 +10620,12 @@
         <v>175.041</v>
       </c>
     </row>
-    <row r="157" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A157" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C157" s="3">
         <v>71.991</v>
@@ -10681,12 +10679,12 @@
         <v>51.344999999999999</v>
       </c>
     </row>
-    <row r="158" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A158" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C158" s="3">
         <v>10847.904</v>
@@ -10740,12 +10738,12 @@
         <v>11012.548000000001</v>
       </c>
     </row>
-    <row r="159" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A159" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C159" s="3">
         <v>112.51900000000001</v>
@@ -10799,12 +10797,12 @@
         <v>86.183000000000007</v>
       </c>
     </row>
-    <row r="160" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A160" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C160" s="3">
         <v>400.12700000000001</v>
@@ -10858,12 +10856,12 @@
         <v>338.66899999999998</v>
       </c>
     </row>
-    <row r="161" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A161" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C161" s="3">
         <v>11402.532999999999</v>
@@ -10917,12 +10915,12 @@
         <v>14760.45</v>
       </c>
     </row>
-    <row r="162" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A162" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C162" s="3">
         <v>2961.1610000000001</v>
@@ -10976,12 +10974,12 @@
         <v>1793.106</v>
       </c>
     </row>
-    <row r="163" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A163" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C163" s="3">
         <v>375.26499999999999</v>
@@ -11035,12 +11033,12 @@
         <v>234.041</v>
       </c>
     </row>
-    <row r="164" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A164" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C164" s="3">
         <v>4.9989999999999997</v>
@@ -11094,12 +11092,12 @@
         <v>2.8780000000000001</v>
       </c>
     </row>
-    <row r="165" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A165" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C165" s="3">
         <v>2860.84</v>
@@ -11153,12 +11151,12 @@
         <v>1216.779</v>
       </c>
     </row>
-    <row r="166" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A166" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C166" s="3">
         <v>9.8849999999999998</v>
@@ -11212,12 +11210,12 @@
         <v>10.138999999999999</v>
       </c>
     </row>
-    <row r="167" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A167" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C167" s="3">
         <v>53.192</v>
@@ -11271,12 +11269,12 @@
         <v>43.395000000000003</v>
       </c>
     </row>
-    <row r="168" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A168" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C168" s="3">
         <v>183.62899999999999</v>
@@ -11330,12 +11328,12 @@
         <v>122.09099999999999</v>
       </c>
     </row>
-    <row r="169" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A169" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C169" s="3">
         <v>38.658999999999999</v>
@@ -11389,12 +11387,12 @@
         <v>60.194000000000003</v>
       </c>
     </row>
-    <row r="170" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A170" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C170" s="3">
         <v>110.947</v>
@@ -11448,12 +11446,12 @@
         <v>74.617999999999995</v>
       </c>
     </row>
-    <row r="171" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A171" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B171" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C171" s="3">
         <v>42.881999999999998</v>
@@ -11507,12 +11505,12 @@
         <v>69.221999999999994</v>
       </c>
     </row>
-    <row r="172" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A172" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C172" s="3">
         <v>1399.491</v>
@@ -11566,12 +11564,12 @@
         <v>968.82600000000002</v>
       </c>
     </row>
-    <row r="173" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A173" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C173" s="3">
         <v>38.718000000000004</v>
@@ -11625,12 +11623,12 @@
         <v>53.609000000000002</v>
       </c>
     </row>
-    <row r="174" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A174" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C174" s="3">
         <v>104.423</v>
@@ -11684,12 +11682,12 @@
         <v>40.462000000000003</v>
       </c>
     </row>
-    <row r="175" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A175" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C175" s="3">
         <v>179670.18599999999</v>
@@ -11743,12 +11741,12 @@
         <v>211854.215</v>
       </c>
     </row>
-    <row r="176" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A176" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C176" s="3">
         <v>397.62099999999998</v>
@@ -11802,12 +11800,12 @@
         <v>620.43899999999996</v>
       </c>
     </row>
-    <row r="177" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A177" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C177" s="3">
         <v>5094.1139999999996</v>
@@ -11861,12 +11859,12 @@
         <v>4797.9690000000001</v>
       </c>
     </row>
-    <row r="178" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A178" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C178" s="3">
         <v>6486.201</v>
@@ -11920,12 +11918,12 @@
         <v>4766.0789999999997</v>
       </c>
     </row>
-    <row r="179" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A179" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C179" s="3">
         <v>17915.566999999999</v>
@@ -11979,12 +11977,12 @@
         <v>31270.073</v>
       </c>
     </row>
-    <row r="180" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A180" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C180" s="3">
         <v>9904.6080000000002</v>
@@ -12038,12 +12036,12 @@
         <v>14325.308999999999</v>
       </c>
     </row>
-    <row r="181" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A181" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C181" s="3">
         <v>128932.753</v>
@@ -12097,12 +12095,12 @@
         <v>141509.94200000001</v>
       </c>
     </row>
-    <row r="182" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A182" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C182" s="3">
         <v>6624.5540000000001</v>
@@ -12156,12 +12154,12 @@
         <v>8124.4049999999997</v>
       </c>
     </row>
-    <row r="183" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A183" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B183" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C183" s="3">
         <v>4314.768</v>
@@ -12215,12 +12213,12 @@
         <v>6439.9989999999998</v>
       </c>
     </row>
-    <row r="184" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A184" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B184" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C184" s="3">
         <v>430759.772</v>
@@ -12274,12 +12272,12 @@
         <v>429300.71600000001</v>
       </c>
     </row>
-    <row r="185" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A185" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B185" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C185" s="3">
         <v>45195.777000000002</v>
@@ -12333,12 +12331,12 @@
         <v>56802.493000000002</v>
       </c>
     </row>
-    <row r="186" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A186" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C186" s="3">
         <v>11673.029</v>
@@ -12392,12 +12390,12 @@
         <v>17390.955999999998</v>
       </c>
     </row>
-    <row r="187" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A187" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C187" s="3">
         <v>212559.40900000001</v>
@@ -12451,12 +12449,12 @@
         <v>180682.76199999999</v>
       </c>
     </row>
-    <row r="188" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A188" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C188" s="3">
         <v>19116.208999999999</v>
@@ -12510,12 +12508,12 @@
         <v>17332.334999999999</v>
       </c>
     </row>
-    <row r="189" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A189" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B189" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C189" s="3">
         <v>50882.883999999998</v>
@@ -12569,12 +12567,12 @@
         <v>45221.275999999998</v>
       </c>
     </row>
-    <row r="190" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A190" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C190" s="3">
         <v>17643.060000000001</v>
@@ -12628,12 +12626,12 @@
         <v>24482.822</v>
       </c>
     </row>
-    <row r="191" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A191" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B191" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C191" s="3">
         <v>3.4830000000000001</v>
@@ -12687,12 +12685,12 @@
         <v>2.7170000000000001</v>
       </c>
     </row>
-    <row r="192" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A192" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C192" s="3">
         <v>298.68200000000002</v>
@@ -12746,12 +12744,12 @@
         <v>927.14300000000003</v>
       </c>
     </row>
-    <row r="193" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A193" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B193" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C193" s="3">
         <v>786.55899999999997</v>
@@ -12805,12 +12803,12 @@
         <v>530.59799999999996</v>
       </c>
     </row>
-    <row r="194" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A194" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B194" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C194" s="3">
         <v>7132.53</v>
@@ -12864,12 +12862,12 @@
         <v>8733.6329999999998</v>
       </c>
     </row>
-    <row r="195" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A195" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B195" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C195" s="3">
         <v>32971.845999999998</v>
@@ -12923,12 +12921,12 @@
         <v>39158.18</v>
       </c>
     </row>
-    <row r="196" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A196" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B196" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C196" s="3">
         <v>586.63400000000001</v>
@@ -12982,12 +12980,12 @@
         <v>613.12199999999996</v>
       </c>
     </row>
-    <row r="197" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A197" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B197" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C197" s="3">
         <v>3473.7269999999999</v>
@@ -13041,12 +13039,12 @@
         <v>3181.9549999999999</v>
       </c>
     </row>
-    <row r="198" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A198" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B198" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C198" s="3">
         <v>28435.942999999999</v>
@@ -13100,12 +13098,12 @@
         <v>34240.724000000002</v>
       </c>
     </row>
-    <row r="199" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A199" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B199" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C199" s="3">
         <v>30322.114000000001</v>
@@ -13159,12 +13157,12 @@
         <v>48885.124000000003</v>
       </c>
     </row>
-    <row r="200" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A200" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B200" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C200" s="3">
         <v>25499.881000000001</v>
@@ -13218,12 +13216,12 @@
         <v>42876.773999999998</v>
       </c>
     </row>
-    <row r="201" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A201" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B201" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C201" s="3">
         <v>4822.2330000000002</v>
@@ -13277,12 +13275,12 @@
         <v>6008.35</v>
       </c>
     </row>
-    <row r="202" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A202" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B202" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C202" s="3">
         <v>12355.695</v>
@@ -13336,12 +13334,12 @@
         <v>26030.486000000001</v>
       </c>
     </row>
-    <row r="203" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A203" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B203" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C203" s="3">
         <v>11122.99</v>
@@ -13395,12 +13393,12 @@
         <v>24583.111000000001</v>
       </c>
     </row>
-    <row r="204" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A204" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B204" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C204" s="3">
         <v>896.44399999999996</v>
@@ -13454,12 +13452,12 @@
         <v>1066.5809999999999</v>
       </c>
     </row>
-    <row r="205" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A205" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B205" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C205" s="3">
         <v>285.49099999999999</v>
@@ -13513,12 +13511,12 @@
         <v>355.99099999999999</v>
       </c>
     </row>
-    <row r="206" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A206" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B206" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C206" s="3">
         <v>8947.027</v>
@@ -13572,12 +13570,12 @@
         <v>19782.704000000002</v>
       </c>
     </row>
-    <row r="207" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A207" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B207" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C207" s="3">
         <v>686.87800000000004</v>
@@ -13631,12 +13629,12 @@
         <v>2409.7669999999998</v>
       </c>
     </row>
-    <row r="208" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A208" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B208" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C208" s="3">
         <v>307.14999999999998</v>
@@ -13690,12 +13688,12 @@
         <v>968.06799999999998</v>
       </c>
     </row>
-    <row r="209" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A209" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B209" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C209" s="3">
         <v>548.92700000000002</v>
@@ -13749,12 +13747,12 @@
         <v>658.77300000000002</v>
       </c>
     </row>
-    <row r="210" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A210" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B210" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C210" s="3">
         <v>168.78299999999999</v>
@@ -13808,12 +13806,12 @@
         <v>167.922</v>
       </c>
     </row>
-    <row r="211" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A211" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B211" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C211" s="3">
         <v>119.446</v>
@@ -13867,12 +13865,12 @@
         <v>239.471</v>
       </c>
     </row>
-    <row r="212" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A212" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B212" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C212" s="3">
         <v>59.194000000000003</v>
@@ -13926,12 +13924,12 @@
         <v>63.210999999999999</v>
       </c>
     </row>
-    <row r="213" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A213" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B213" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C213" s="3">
         <v>115.021</v>
@@ -13985,12 +13983,12 @@
         <v>114.73399999999999</v>
       </c>
     </row>
-    <row r="214" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A214" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B214" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C214" s="3">
         <v>10.834</v>
@@ -14044,12 +14042,12 @@
         <v>5.7939999999999996</v>
       </c>
     </row>
-    <row r="215" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A215" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B215" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C215" s="3">
         <v>57.557000000000002</v>
@@ -14103,12 +14101,12 @@
         <v>53.39</v>
       </c>
     </row>
-    <row r="216" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A216" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C216" s="3">
         <v>18.091999999999999</v>
@@ -14162,12 +14160,12 @@
         <v>14.250999999999999</v>
       </c>
     </row>
-    <row r="217" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A217" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B217" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C217" s="3">
         <v>683.77800000000002</v>
@@ -14221,12 +14219,12 @@
         <v>788.60199999999998</v>
       </c>
     </row>
-    <row r="218" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A218" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B218" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C218" s="3">
         <v>55.197000000000003</v>
@@ -14280,12 +14278,12 @@
         <v>36.155999999999999</v>
       </c>
     </row>
-    <row r="219" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A219" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B219" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C219" s="3">
         <v>17.564</v>
@@ -14339,12 +14337,12 @@
         <v>13.786</v>
       </c>
     </row>
-    <row r="220" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A220" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B220" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C220" s="3">
         <v>280.904</v>
@@ -14398,12 +14396,12 @@
         <v>261.54500000000002</v>
       </c>
     </row>
-    <row r="221" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A221" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B221" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C221" s="3">
         <v>1.6180000000000001</v>
@@ -14457,12 +14455,12 @@
         <v>1.726</v>
       </c>
     </row>
-    <row r="222" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A222" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B222" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C222" s="3">
         <v>198.41</v>
@@ -14516,12 +14514,12 @@
         <v>310.10599999999999</v>
       </c>
     </row>
-    <row r="223" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A223" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B223" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C223" s="3">
         <v>1.35</v>
@@ -14575,12 +14573,12 @@
         <v>1.456</v>
       </c>
     </row>
-    <row r="224" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A224" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C224" s="3">
         <v>105.697</v>
@@ -14634,12 +14632,12 @@
         <v>138.261</v>
       </c>
     </row>
-    <row r="225" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A225" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B225" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C225" s="3">
         <v>11.792</v>
@@ -14693,12 +14691,12 @@
         <v>20.007999999999999</v>
       </c>
     </row>
-    <row r="226" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A226" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C226" s="3">
         <v>11.246</v>
@@ -14752,12 +14750,12 @@
         <v>5.5579999999999998</v>
       </c>
     </row>
-    <row r="227" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A227" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B227" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C227" s="3">
         <v>1116505.689</v>
@@ -14811,12 +14809,12 @@
         <v>1120451.118</v>
       </c>
     </row>
-    <row r="228" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A228" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B228" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C228" s="3">
         <v>747636.04500000004</v>
@@ -14870,12 +14868,12 @@
         <v>629562.56200000003</v>
       </c>
     </row>
-    <row r="229" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A229" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B229" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C229" s="3">
         <v>293013.21000000002</v>
@@ -14929,12 +14927,12 @@
         <v>219456.41200000001</v>
       </c>
     </row>
-    <row r="230" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="230" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A230" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B230" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C230" s="3">
         <v>9449.3209999999999</v>
@@ -14988,12 +14986,12 @@
         <v>7429.6729999999998</v>
       </c>
     </row>
-    <row r="231" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="231" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A231" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B231" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C231" s="3">
         <v>6948.4449999999997</v>
@@ -15047,12 +15045,12 @@
         <v>3588.337</v>
       </c>
     </row>
-    <row r="232" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="232" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A232" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B232" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C232" s="3">
         <v>10708.982</v>
@@ -15106,12 +15104,12 @@
         <v>10274.07</v>
       </c>
     </row>
-    <row r="233" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="233" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A233" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B233" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C233" s="3">
         <v>9660.35</v>
@@ -15165,12 +15163,12 @@
         <v>6856.92</v>
       </c>
     </row>
-    <row r="234" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="234" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A234" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B234" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C234" s="3">
         <v>37846.605000000003</v>
@@ -15224,12 +15222,12 @@
         <v>23032.569</v>
       </c>
     </row>
-    <row r="235" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="235" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A235" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C235" s="3">
         <v>4033.9630000000002</v>
@@ -15283,12 +15281,12 @@
         <v>2011.568</v>
       </c>
     </row>
-    <row r="236" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="236" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A236" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B236" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C236" s="3">
         <v>19237.682000000001</v>
@@ -15342,12 +15340,12 @@
         <v>11877.960999999999</v>
       </c>
     </row>
-    <row r="237" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="237" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A237" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B237" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C237" s="3">
         <v>145934.46</v>
@@ -15401,12 +15399,12 @@
         <v>126142.651</v>
       </c>
     </row>
-    <row r="238" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="238" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A238" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B238" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C238" s="3">
         <v>5459.643</v>
@@ -15460,12 +15458,12 @@
         <v>3829.2109999999998</v>
       </c>
     </row>
-    <row r="239" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="239" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A239" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B239" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C239" s="3">
         <v>43733.758999999998</v>
@@ -15519,12 +15517,12 @@
         <v>24413.452000000001</v>
       </c>
     </row>
-    <row r="240" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="240" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A240" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B240" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C240" s="3">
         <v>106261.27099999999</v>
@@ -15578,12 +15576,12 @@
         <v>121044.272</v>
       </c>
     </row>
-    <row r="241" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="241" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A241" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B241" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C241" s="3">
         <v>173.85900000000001</v>
@@ -15637,12 +15635,12 @@
         <v>222.51400000000001</v>
       </c>
     </row>
-    <row r="242" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="242" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A242" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B242" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C242" s="3">
         <v>5792.2030000000004</v>
@@ -15696,12 +15694,12 @@
         <v>6872.9070000000002</v>
       </c>
     </row>
-    <row r="243" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="243" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A243" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B243" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C243" s="3">
         <v>1326.539</v>
@@ -15755,12 +15753,12 @@
         <v>837.72</v>
       </c>
     </row>
-    <row r="244" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="244" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A244" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B244" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C244" s="3">
         <v>48.865000000000002</v>
@@ -15814,12 +15812,12 @@
         <v>55.097000000000001</v>
       </c>
     </row>
-    <row r="245" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="245" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A245" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B245" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C245" s="3">
         <v>5540.7179999999998</v>
@@ -15873,12 +15871,12 @@
         <v>5254.37</v>
       </c>
     </row>
-    <row r="246" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="246" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A246" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B246" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C246" s="3">
         <v>341.25</v>
@@ -15932,12 +15930,12 @@
         <v>353.291</v>
       </c>
     </row>
-    <row r="247" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="247" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A247" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B247" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C247" s="3">
         <v>4937.7960000000003</v>
@@ -15991,12 +15989,12 @@
         <v>5684.9620000000004</v>
       </c>
     </row>
-    <row r="248" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="248" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A248" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B248" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C248" s="3">
         <v>85.031999999999996</v>
@@ -16050,12 +16048,12 @@
         <v>96.201999999999998</v>
       </c>
     </row>
-    <row r="249" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="249" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A249" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B249" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C249" s="3">
         <v>1886.202</v>
@@ -16109,12 +16107,12 @@
         <v>1114.4010000000001</v>
       </c>
     </row>
-    <row r="250" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="250" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A250" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B250" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C250" s="3">
         <v>2722.2910000000002</v>
@@ -16168,12 +16166,12 @@
         <v>1524.086</v>
       </c>
     </row>
-    <row r="251" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="251" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A251" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B251" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C251" s="3">
         <v>5421.2420000000002</v>
@@ -16227,12 +16225,12 @@
         <v>7952.9269999999997</v>
       </c>
     </row>
-    <row r="252" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="252" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A252" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B252" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C252" s="3">
         <v>10099.27</v>
@@ -16286,12 +16284,12 @@
         <v>13022.531999999999</v>
       </c>
     </row>
-    <row r="253" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="253" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A253" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B253" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C253" s="3">
         <v>67886.004000000001</v>
@@ -16345,12 +16343,12 @@
         <v>78053.263000000006</v>
       </c>
     </row>
-    <row r="254" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="254" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A254" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B254" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C254" s="3">
         <v>152215.24299999999</v>
@@ -16404,12 +16402,12 @@
         <v>99758.366999999998</v>
       </c>
     </row>
-    <row r="255" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="255" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A255" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C255" s="3">
         <v>2877.8</v>
@@ -16463,12 +16461,12 @@
         <v>1088.338</v>
       </c>
     </row>
-    <row r="256" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="256" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A256" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B256" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C256" s="3">
         <v>77.265000000000001</v>
@@ -16522,12 +16520,12 @@
         <v>62.405999999999999</v>
       </c>
     </row>
-    <row r="257" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="257" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A257" s="13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B257" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C257" s="3">
         <v>3280.8150000000001</v>
@@ -16581,12 +16579,12 @@
         <v>1641.0540000000001</v>
       </c>
     </row>
-    <row r="258" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="258" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A258" s="13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B258" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C258" s="3">
         <v>4105.268</v>
@@ -16640,12 +16638,12 @@
         <v>2183.3139999999999</v>
       </c>
     </row>
-    <row r="259" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="259" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A259" s="13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B259" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C259" s="3">
         <v>33.691000000000003</v>
@@ -16699,12 +16697,12 @@
         <v>27.242000000000001</v>
       </c>
     </row>
-    <row r="260" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="260" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A260" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B260" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C260" s="3">
         <v>10423.056</v>
@@ -16758,12 +16756,12 @@
         <v>6583.3639999999996</v>
       </c>
     </row>
-    <row r="261" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="261" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A261" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B261" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C261" s="3">
         <v>0.80900000000000005</v>
@@ -16817,12 +16815,12 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="262" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="262" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A262" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B262" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C262" s="3">
         <v>60461.828000000001</v>
@@ -16876,12 +16874,12 @@
         <v>39992.910000000003</v>
       </c>
     </row>
-    <row r="263" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="263" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A263" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B263" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C263" s="3">
         <v>441.53899999999999</v>
@@ -16935,12 +16933,12 @@
         <v>357.73200000000003</v>
       </c>
     </row>
-    <row r="264" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="264" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A264" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B264" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C264" s="3">
         <v>628.06200000000001</v>
@@ -16994,12 +16992,12 @@
         <v>453.65600000000001</v>
       </c>
     </row>
-    <row r="265" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="265" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A265" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B265" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C265" s="3">
         <v>2083.38</v>
@@ -17053,12 +17051,12 @@
         <v>1249.3610000000001</v>
       </c>
     </row>
-    <row r="266" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="266" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A266" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B266" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C266" s="3">
         <v>10196.707</v>
@@ -17112,12 +17110,12 @@
         <v>6984.9549999999999</v>
       </c>
     </row>
-    <row r="267" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="267" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A267" s="13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B267" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C267" s="3">
         <v>33.938000000000002</v>
@@ -17171,12 +17169,12 @@
         <v>29.693000000000001</v>
       </c>
     </row>
-    <row r="268" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="268" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A268" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B268" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C268" s="3">
         <v>8737.3700000000008</v>
@@ -17230,12 +17228,12 @@
         <v>4217.4250000000002</v>
       </c>
     </row>
-    <row r="269" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="269" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A269" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B269" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C269" s="3">
         <v>2078.9319999999998</v>
@@ -17289,12 +17287,12 @@
         <v>1676.2639999999999</v>
       </c>
     </row>
-    <row r="270" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="270" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A270" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B270" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C270" s="3">
         <v>46754.783000000003</v>
@@ -17348,12 +17346,12 @@
         <v>33209.856</v>
       </c>
     </row>
-    <row r="271" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="271" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A271" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B271" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C271" s="3">
         <v>196146.321</v>
@@ -17407,12 +17405,12 @@
         <v>189303.511</v>
       </c>
     </row>
-    <row r="272" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="272" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A272" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B272" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C272" s="3">
         <v>9006.4</v>
@@ -17466,12 +17464,12 @@
         <v>8676.8439999999991</v>
       </c>
     </row>
-    <row r="273" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="273" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A273" s="13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B273" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C273" s="3">
         <v>11589.616</v>
@@ -17525,12 +17523,12 @@
         <v>12492.831</v>
       </c>
     </row>
-    <row r="274" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="274" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A274" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B274" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C274" s="3">
         <v>65273.512000000002</v>
@@ -17584,12 +17582,12 @@
         <v>65497.773000000001</v>
       </c>
     </row>
-    <row r="275" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="275" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A275" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B275" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C275" s="3">
         <v>83783.945000000007</v>
@@ -17643,12 +17641,12 @@
         <v>74740.596000000005</v>
       </c>
     </row>
-    <row r="276" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="276" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A276" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B276" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C276" s="3">
         <v>38.137</v>
@@ -17702,12 +17700,12 @@
         <v>45.212000000000003</v>
       </c>
     </row>
-    <row r="277" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="277" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A277" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B277" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C277" s="3">
         <v>625.976</v>
@@ -17761,12 +17759,12 @@
         <v>985.16800000000001</v>
       </c>
     </row>
-    <row r="278" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="278" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A278" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B278" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C278" s="3">
         <v>39.244</v>
@@ -17820,12 +17818,12 @@
         <v>64.364999999999995</v>
       </c>
     </row>
-    <row r="279" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="279" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A279" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B279" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C279" s="3">
         <v>17134.873</v>
@@ -17879,12 +17877,12 @@
         <v>15759.617</v>
       </c>
     </row>
-    <row r="280" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="280" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A280" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B280" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C280" s="3">
         <v>8654.6180000000004</v>
@@ -17938,12 +17936,12 @@
         <v>11041.105</v>
       </c>
     </row>
-    <row r="281" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="281" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A281" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B281" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C281" s="3">
         <v>368869.64399999997</v>
@@ -17997,12 +17995,12 @@
         <v>490888.55599999998</v>
       </c>
     </row>
-    <row r="282" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="282" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A282" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B282" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C282" s="3">
         <v>62.273000000000003</v>
@@ -18056,12 +18054,12 @@
         <v>36.933</v>
       </c>
     </row>
-    <row r="283" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="283" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A283" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B283" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C283" s="3">
         <v>37742.156999999999</v>
@@ -18115,12 +18113,12 @@
         <v>56953.224000000002</v>
       </c>
     </row>
-    <row r="284" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="284" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A284" s="11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B284" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C284" s="3">
         <v>56.771999999999998</v>
@@ -18174,12 +18172,12 @@
         <v>40.524000000000001</v>
       </c>
     </row>
-    <row r="285" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="285" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A285" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B285" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C285" s="3">
         <v>5.7949999999999999</v>
@@ -18233,12 +18231,12 @@
         <v>3.984</v>
       </c>
     </row>
-    <row r="286" spans="1:19" ht="12" x14ac:dyDescent="0.15">
+    <row r="286" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A286" s="11" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B286" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C286" s="3">
         <v>331002.647</v>

</xml_diff>